<commit_message>
Latest changes in original Spring 2023 branch and changes in Timer class
</commit_message>
<xml_diff>
--- a/INFO6205/Assignment2/Assignment2_002772160.xlsx
+++ b/INFO6205/Assignment2/Assignment2_002772160.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivanidatar/Documents/6205/PSA-Git/info6205-psa/INFO6205/Assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC0BA83-2666-FC40-84E5-33A2FE2EB3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2304C4E-0FDF-6D4F-A4A8-513CD0A8F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17200" xr2:uid="{9BE36209-CEBA-8A46-A923-76A25FA9FF80}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>N</t>
   </si>
@@ -5510,10 +5510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0652324E-9C2B-1C43-B0BB-047EA06BDF6E}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="A21" sqref="A21:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5521,9 +5521,10 @@
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5536,8 +5537,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>250</v>
       </c>
@@ -5550,8 +5554,11 @@
       <c r="D2">
         <v>6.2</v>
       </c>
+      <c r="E2">
+        <v>0.91</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>500</v>
       </c>
@@ -5564,8 +5571,11 @@
       <c r="D3">
         <v>47.24</v>
       </c>
+      <c r="E3">
+        <v>0.83</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -5578,8 +5588,11 @@
       <c r="D4">
         <v>373.85</v>
       </c>
+      <c r="E4">
+        <v>4.88</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2000</v>
       </c>
@@ -5592,8 +5605,11 @@
       <c r="D5">
         <v>2976.02</v>
       </c>
+      <c r="E5">
+        <v>20.190000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4000</v>
       </c>
@@ -5606,8 +5622,11 @@
       <c r="D6">
         <v>23723.9</v>
       </c>
+      <c r="E6">
+        <v>146.44</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8000</v>
       </c>
@@ -5620,8 +5639,11 @@
       <c r="D7">
         <v>189171.99</v>
       </c>
+      <c r="E7">
+        <v>616.52</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16000</v>
       </c>
@@ -5631,8 +5653,11 @@
       <c r="C8">
         <v>8953.6200000000008</v>
       </c>
+      <c r="E8">
+        <v>3419.62</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -5640,7 +5665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>250</v>
       </c>
@@ -5648,7 +5673,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>500</v>
       </c>
@@ -5656,7 +5681,7 @@
         <v>3.23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1000</v>
       </c>
@@ -5664,7 +5689,7 @@
         <v>17.260000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2000</v>
       </c>
@@ -5672,7 +5697,7 @@
         <v>86.9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4000</v>
       </c>

</xml_diff>